<commit_message>
250217_Laptop to PC arrival
</commit_message>
<xml_diff>
--- a/RGGI PnL Output.xlsx
+++ b/RGGI PnL Output.xlsx
@@ -479,16 +479,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>261686.8399545376</v>
+        <v>337818.8581867374</v>
       </c>
       <c r="E2" t="n">
-        <v>-569032.4677793727</v>
+        <v>-688063.8732537836</v>
       </c>
     </row>
     <row r="3">
@@ -496,16 +496,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>261625.678036339</v>
+        <v>334113.820859102</v>
       </c>
       <c r="E3" t="n">
-        <v>-504193.6837808596</v>
+        <v>-604903.3109674883</v>
       </c>
     </row>
     <row r="4">
@@ -513,16 +513,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>261280.9393927187</v>
+        <v>325402.4147817142</v>
       </c>
       <c r="E4" t="n">
-        <v>-439638.4765077682</v>
+        <v>-526749.1174309454</v>
       </c>
     </row>
     <row r="5">
@@ -530,16 +530,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>259947.1335963028</v>
+        <v>309124.3417766306</v>
       </c>
       <c r="E5" t="n">
-        <v>-376072.3363874723</v>
+        <v>-456161.5908220985</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>256123.5809792298</v>
+        <v>283775.3130786944</v>
       </c>
       <c r="E6" t="n">
-        <v>-314995.9430878336</v>
+        <v>-394645.019906104</v>
       </c>
     </row>
     <row r="7">
@@ -564,16 +564,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>247514.5953076935</v>
+        <v>249692.9071364171</v>
       </c>
       <c r="E7" t="n">
-        <v>-258704.9828426582</v>
+        <v>-341861.8262344506</v>
       </c>
     </row>
     <row r="8">
@@ -581,16 +581,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>231606.9079603206</v>
+        <v>209057.2053564017</v>
       </c>
       <c r="E8" t="n">
-        <v>-209712.7242733192</v>
+        <v>-295631.9284005354</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>206712.2951161415</v>
+        <v>165206.9639242061</v>
       </c>
       <c r="E9" t="n">
-        <v>-169707.3912007866</v>
+        <v>-252616.5702188003</v>
       </c>
     </row>
     <row r="10">
@@ -615,16 +615,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>173015.0444467223</v>
+        <v>121693.0553759176</v>
       </c>
       <c r="E10" t="n">
-        <v>-138504.695953494</v>
+        <v>-209264.8791531582</v>
       </c>
     </row>
     <row r="11">
@@ -632,16 +632,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>133030.9998471866</v>
+        <v>81482.46711378793</v>
       </c>
       <c r="E11" t="n">
-        <v>-113588.794636318</v>
+        <v>-162609.8678013571</v>
       </c>
     </row>
     <row r="12">
@@ -649,16 +649,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>91071.50211057202</v>
+        <v>46527.40230091067</v>
       </c>
       <c r="E12" t="n">
-        <v>-90648.34645622088</v>
+        <v>-110699.3330003037</v>
       </c>
     </row>
     <row r="13">
@@ -666,16 +666,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>51856.1725160486</v>
+        <v>17704.19950159836</v>
       </c>
       <c r="E13" t="n">
-        <v>-64963.73013403257</v>
+        <v>-52656.93618568538</v>
       </c>
     </row>
     <row r="14">
@@ -683,16 +683,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>18996.73854435059</v>
+        <v>-4996.284614053426</v>
       </c>
       <c r="E14" t="n">
-        <v>-32923.21818901884</v>
+        <v>11508.17931259351</v>
       </c>
     </row>
     <row r="15">
@@ -700,16 +700,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-5861.125829113435</v>
+        <v>-22172.01938797691</v>
       </c>
       <c r="E15" t="n">
-        <v>7118.863354228868</v>
+        <v>81198.04415260069</v>
       </c>
     </row>
     <row r="16">
@@ -717,16 +717,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-22961.86949912143</v>
+        <v>-34718.88572413799</v>
       </c>
       <c r="E16" t="n">
-        <v>54918.0656009326</v>
+        <v>155516.7774303703</v>
       </c>
     </row>
     <row r="17">
@@ -734,16 +734,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-33738.61483044877</v>
+        <v>-43605.67827144285</v>
       </c>
       <c r="E17" t="n">
-        <v>109041.266186317</v>
+        <v>233495.584496996</v>
       </c>
     </row>
     <row r="18">
@@ -751,16 +751,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-40004.2358118536</v>
+        <v>-49731.2463212224</v>
       </c>
       <c r="E18" t="n">
-        <v>167675.5911216239</v>
+        <v>314235.6160611472</v>
       </c>
     </row>
     <row r="19">
@@ -768,16 +768,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-43387.49045235405</v>
+        <v>-53853.49424606087</v>
       </c>
       <c r="E19" t="n">
-        <v>229192.2823978352</v>
+        <v>396978.9677502393</v>
       </c>
     </row>
     <row r="20">
@@ -785,16 +785,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-45094.42716526178</v>
+        <v>-56569.48821683889</v>
       </c>
       <c r="E20" t="n">
-        <v>292385.2916016392</v>
+        <v>481128.573393392</v>
       </c>
     </row>
     <row r="21">
@@ -802,16 +802,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-45903.31752948246</v>
+        <v>-58325.80453564587</v>
       </c>
       <c r="E21" t="n">
-        <v>356476.3471541302</v>
+        <v>566237.8566885156</v>
       </c>
     </row>
     <row r="22">
@@ -819,16 +819,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46264.90542674638</v>
+        <v>-59442.92795315228</v>
       </c>
       <c r="E22" t="n">
-        <v>421014.705173578</v>
+        <v>651986.3328849399</v>
       </c>
     </row>
     <row r="23">
@@ -836,16 +836,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46417.84992973667</v>
+        <v>-60143.18866558684</v>
       </c>
       <c r="E23" t="n">
-        <v>485761.7065872995</v>
+        <v>738151.671786436</v>
       </c>
     </row>
     <row r="24">
@@ -853,16 +853,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46479.1556133678</v>
+        <v>-60576.51923595641</v>
       </c>
       <c r="E24" t="n">
-        <v>550600.3468203801</v>
+        <v>824583.9408299973</v>
       </c>
     </row>
     <row r="25">
@@ -870,16 +870,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46502.42304828514</v>
+        <v>-60841.6365051256</v>
       </c>
       <c r="E25" t="n">
-        <v>615477.0253021745</v>
+        <v>911184.4231747587</v>
       </c>
     </row>
     <row r="26">
@@ -887,16 +887,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46510.74513763019</v>
+        <v>-61002.22034037028</v>
       </c>
       <c r="E26" t="n">
-        <v>680368.6491295412</v>
+        <v>997889.4389534447</v>
       </c>
     </row>
     <row r="27">
@@ -904,16 +904,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46513.51666187705</v>
+        <v>-61098.63287811747</v>
       </c>
       <c r="E27" t="n">
-        <v>745265.823522006</v>
+        <v>1084658.626029628</v>
       </c>
     </row>
     <row r="28">
@@ -921,16 +921,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.35170327536</v>
+        <v>-61156.07100524566</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.9343973196</v>
+        <v>1171466.78751643</v>
       </c>
     </row>
     <row r="29">
@@ -938,16 +938,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.56199105312</v>
+        <v>-61190.05859093236</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6700262536</v>
+        <v>1258298.399544675</v>
       </c>
     </row>
     <row r="30">
@@ -955,16 +955,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.59299779098</v>
+        <v>-61210.05116072671</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.5849362274</v>
+        <v>1345144.006588811</v>
       </c>
     </row>
     <row r="31">
@@ -972,16 +972,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.58336569626</v>
+        <v>-61221.75105322598</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.540485034</v>
+        <v>1431997.906310242</v>
       </c>
     </row>
     <row r="32">
@@ -989,16 +989,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.57055785255</v>
+        <v>-61228.56757438225</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.499209589</v>
+        <v>1518856.689403017</v>
       </c>
     </row>
   </sheetData>
@@ -1052,16 +1052,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262053.1760176996</v>
+        <v>340233.8867747966</v>
       </c>
       <c r="E2" t="n">
-        <v>-568666.1317162106</v>
+        <v>-685648.8446657243</v>
       </c>
     </row>
     <row r="3">
@@ -1069,16 +1069,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262052.1290307638</v>
+        <v>339966.2538623855</v>
       </c>
       <c r="E3" t="n">
-        <v>-503767.2327864348</v>
+        <v>-599050.8779642048</v>
       </c>
     </row>
     <row r="4">
@@ -1086,16 +1086,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262033.2374805394</v>
+        <v>338178.4296195019</v>
       </c>
       <c r="E4" t="n">
-        <v>-438886.1784199474</v>
+        <v>-513973.1025931577</v>
       </c>
     </row>
     <row r="5">
@@ -1103,16 +1103,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>261854.3471830526</v>
+        <v>331191.9111831858</v>
       </c>
       <c r="E5" t="n">
-        <v>-374165.1228007225</v>
+        <v>-434094.0214155433</v>
       </c>
     </row>
     <row r="6">
@@ -1120,16 +1120,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>260843.1266336999</v>
+        <v>313183.8741813278</v>
       </c>
       <c r="E6" t="n">
-        <v>-310276.3974333635</v>
+        <v>-365236.4588034706</v>
       </c>
     </row>
     <row r="7">
@@ -1137,16 +1137,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>257070.6639807117</v>
+        <v>279533.0266228882</v>
       </c>
       <c r="E7" t="n">
-        <v>-249148.91416964</v>
+        <v>-312021.7067479794</v>
       </c>
     </row>
     <row r="8">
@@ -1154,16 +1154,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>247007.5159597138</v>
+        <v>230457.5151920661</v>
       </c>
       <c r="E8" t="n">
-        <v>-194312.116273926</v>
+        <v>-274231.618564871</v>
       </c>
     </row>
     <row r="9">
@@ -1171,16 +1171,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>226537.5169432924</v>
+        <v>171469.7645637202</v>
       </c>
       <c r="E9" t="n">
-        <v>-149882.1693736357</v>
+        <v>-246353.7695792862</v>
       </c>
     </row>
     <row r="10">
@@ -1188,16 +1188,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>193183.4696042937</v>
+        <v>110839.5598289886</v>
       </c>
       <c r="E10" t="n">
-        <v>-118336.2707959227</v>
+        <v>-220118.3747000872</v>
       </c>
     </row>
     <row r="11">
@@ -1205,16 +1205,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>148215.4515636665</v>
+        <v>56332.50891680951</v>
       </c>
       <c r="E11" t="n">
-        <v>-98404.34291983815</v>
+        <v>-187759.8259983356</v>
       </c>
     </row>
     <row r="12">
@@ -1222,16 +1222,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>97254.70540587198</v>
+        <v>12893.63287926742</v>
       </c>
       <c r="E12" t="n">
-        <v>-84465.14316092092</v>
+        <v>-144333.102421947</v>
       </c>
     </row>
     <row r="13">
@@ -1239,16 +1239,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>48503.81527738606</v>
+        <v>-18072.45204422124</v>
       </c>
       <c r="E13" t="n">
-        <v>-68316.08737269511</v>
+        <v>-88433.58773150497</v>
       </c>
     </row>
     <row r="14">
@@ -1256,16 +1256,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>9123.069623418985</v>
+        <v>-37970.36615482749</v>
       </c>
       <c r="E14" t="n">
-        <v>-42796.88710995045</v>
+        <v>-21465.90222818055</v>
       </c>
     </row>
     <row r="15">
@@ -1273,16 +1273,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-17791.82062481192</v>
+        <v>-49583.49484155778</v>
       </c>
       <c r="E15" t="n">
-        <v>-4811.831441469621</v>
+        <v>53786.56869901982</v>
       </c>
     </row>
     <row r="16">
@@ -1290,16 +1290,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-33441.20463619945</v>
+        <v>-55787.94184645047</v>
       </c>
       <c r="E16" t="n">
-        <v>44438.73046385458</v>
+        <v>134447.7213080578</v>
       </c>
     </row>
     <row r="17">
@@ -1307,16 +1307,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-41248.86624254913</v>
+        <v>-58846.20301431746</v>
       </c>
       <c r="E17" t="n">
-        <v>101531.0147742166</v>
+        <v>218255.0597541214</v>
       </c>
     </row>
     <row r="18">
@@ -1324,16 +1324,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-44626.3515538549</v>
+        <v>-60247.65880251475</v>
       </c>
       <c r="E18" t="n">
-        <v>163053.4753796226</v>
+        <v>303719.2035798548</v>
       </c>
     </row>
     <row r="19">
@@ -1341,16 +1341,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-45907.3855623303</v>
+        <v>-60849.0576080773</v>
       </c>
       <c r="E19" t="n">
-        <v>226672.3872878589</v>
+        <v>389983.4043882229</v>
       </c>
     </row>
     <row r="20">
@@ -1358,16 +1358,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46338.14115470149</v>
+        <v>-61092.3621754741</v>
       </c>
       <c r="E20" t="n">
-        <v>291141.5776121995</v>
+        <v>476605.6994347568</v>
       </c>
     </row>
     <row r="21">
@@ -1375,16 +1375,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46467.90128933441</v>
+        <v>-61185.73683227707</v>
       </c>
       <c r="E21" t="n">
-        <v>355911.7633942783</v>
+        <v>563377.9243918845</v>
       </c>
     </row>
     <row r="22">
@@ -1392,16 +1392,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46503.25182841415</v>
+        <v>-61219.92243662559</v>
       </c>
       <c r="E22" t="n">
-        <v>420776.3587719103</v>
+        <v>650209.3384014666</v>
       </c>
     </row>
     <row r="23">
@@ -1409,16 +1409,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46512.03243658371</v>
+        <v>-61231.92307078643</v>
       </c>
       <c r="E23" t="n">
-        <v>485667.5240804525</v>
+        <v>737062.9373812365</v>
       </c>
     </row>
     <row r="24">
@@ -1426,16 +1426,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.03366247116</v>
+        <v>-61235.98100266679</v>
       </c>
       <c r="E24" t="n">
-        <v>550565.4687712768</v>
+        <v>823924.4790632869</v>
       </c>
     </row>
     <row r="25">
@@ -1443,16 +1443,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.45380082766</v>
+        <v>-61237.30820547065</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.9945496321</v>
+        <v>910788.7514744136</v>
       </c>
     </row>
     <row r="26">
@@ -1460,16 +1460,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.53503331613</v>
+        <v>-61237.7296224501</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8592338553</v>
+        <v>997653.929671365</v>
       </c>
     </row>
     <row r="27">
@@ -1477,16 +1477,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.54938402827</v>
+        <v>-61237.85996164282</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7907998548</v>
+        <v>1084519.398946103</v>
       </c>
     </row>
     <row r="28">
@@ -1494,16 +1494,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55164169545</v>
+        <v>-61237.89934611997</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7344588995</v>
+        <v>1171384.959175556</v>
       </c>
     </row>
     <row r="29">
@@ -1511,16 +1511,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55193349301</v>
+        <v>-61237.91100426073</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800838137</v>
+        <v>1258250.547131346</v>
       </c>
     </row>
     <row r="30">
@@ -1528,16 +1528,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55195418894</v>
+        <v>-61237.91439299194</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259798295</v>
+        <v>1345116.143356546</v>
       </c>
     </row>
     <row r="31">
@@ -1545,16 +1545,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194987044</v>
+        <v>-61237.91536236976</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.57190086</v>
+        <v>1431981.742001099</v>
       </c>
     </row>
     <row r="32">
@@ -1562,16 +1562,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194713772</v>
+        <v>-61237.91563580096</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.517820304</v>
+        <v>1518847.341341598</v>
       </c>
     </row>
   </sheetData>
@@ -1625,16 +1625,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -1642,16 +1642,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -1659,16 +1659,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -1676,16 +1676,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -1693,16 +1693,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -1710,16 +1710,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -1727,16 +1727,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -1744,16 +1744,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -1761,16 +1761,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -1778,16 +1778,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -1795,16 +1795,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -1812,16 +1812,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -1829,16 +1829,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -1846,16 +1846,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -1863,16 +1863,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -1880,16 +1880,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -1897,16 +1897,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -1914,16 +1914,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -1931,16 +1931,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -1948,16 +1948,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -1965,16 +1965,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -1982,16 +1982,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -1999,16 +1999,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -2016,16 +2016,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -2033,16 +2033,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -2050,16 +2050,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -2067,16 +2067,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -2084,16 +2084,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -2101,16 +2101,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -2118,16 +2118,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -2135,16 +2135,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>
@@ -2198,16 +2198,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -2215,16 +2215,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -2232,16 +2232,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -2249,16 +2249,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -2266,16 +2266,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -2283,16 +2283,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -2300,16 +2300,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -2317,16 +2317,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -2334,16 +2334,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -2351,16 +2351,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -2368,16 +2368,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -2385,16 +2385,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -2402,16 +2402,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -2419,16 +2419,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -2436,16 +2436,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -2453,16 +2453,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -2470,16 +2470,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -2487,16 +2487,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -2504,16 +2504,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -2521,16 +2521,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -2538,16 +2538,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -2555,16 +2555,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -2572,16 +2572,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -2589,16 +2589,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -2606,16 +2606,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -2623,16 +2623,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -2640,16 +2640,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -2657,16 +2657,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -2674,16 +2674,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -2691,16 +2691,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -2708,16 +2708,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>
@@ -2771,16 +2771,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -2788,16 +2788,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -2805,16 +2805,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -2822,16 +2822,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -2839,16 +2839,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -2856,16 +2856,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -2873,16 +2873,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -2890,16 +2890,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -2907,16 +2907,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -2924,16 +2924,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -2941,16 +2941,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -2958,16 +2958,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -2975,16 +2975,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -2992,16 +2992,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -3009,16 +3009,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -3026,16 +3026,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -3043,16 +3043,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -3060,16 +3060,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -3077,16 +3077,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -3094,16 +3094,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -3111,16 +3111,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -3128,16 +3128,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -3145,16 +3145,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -3162,16 +3162,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -3179,16 +3179,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -3196,16 +3196,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -3213,16 +3213,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -3230,16 +3230,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -3247,16 +3247,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -3264,16 +3264,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -3281,16 +3281,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>
@@ -3344,16 +3344,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -3361,16 +3361,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -3378,16 +3378,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -3395,16 +3395,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -3412,16 +3412,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -3429,16 +3429,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -3446,16 +3446,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -3463,16 +3463,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -3480,16 +3480,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -3497,16 +3497,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -3514,16 +3514,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -3531,16 +3531,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -3548,16 +3548,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -3565,16 +3565,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -3582,16 +3582,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -3599,16 +3599,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -3616,16 +3616,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -3633,16 +3633,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -3650,16 +3650,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -3667,16 +3667,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -3684,16 +3684,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -3701,16 +3701,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -3718,16 +3718,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -3735,16 +3735,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -3752,16 +3752,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -3769,16 +3769,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -3786,16 +3786,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -3803,16 +3803,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -3820,16 +3820,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -3837,16 +3837,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -3854,16 +3854,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>
@@ -3917,16 +3917,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -3934,16 +3934,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -3951,16 +3951,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -3968,16 +3968,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -3985,16 +3985,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -4002,16 +4002,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -4019,16 +4019,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -4036,16 +4036,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -4053,16 +4053,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -4070,16 +4070,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -4087,16 +4087,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -4104,16 +4104,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -4121,16 +4121,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -4138,16 +4138,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -4155,16 +4155,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -4172,16 +4172,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -4189,16 +4189,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -4206,16 +4206,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -4223,16 +4223,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -4240,16 +4240,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -4257,16 +4257,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -4274,16 +4274,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -4291,16 +4291,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -4308,16 +4308,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -4325,16 +4325,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -4342,16 +4342,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -4359,16 +4359,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -4376,16 +4376,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -4393,16 +4393,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -4410,16 +4410,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -4427,16 +4427,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>
@@ -4490,16 +4490,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-830719.3077339103</v>
+        <v>-1025882.731440521</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E2" t="n">
-        <v>-568186.4981715404</v>
+        <v>-684965.0934131721</v>
       </c>
     </row>
     <row r="3">
@@ -4507,16 +4507,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-765819.3618171986</v>
+        <v>-939017.1318265903</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E3" t="n">
-        <v>-503286.5522548287</v>
+        <v>-598099.4937992413</v>
       </c>
     </row>
     <row r="4">
@@ -4524,16 +4524,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-700919.4159004869</v>
+        <v>-852151.5322126596</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>262532.8095623697</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E4" t="n">
-        <v>-438386.6063381172</v>
+        <v>-511233.8941853106</v>
       </c>
     </row>
     <row r="5">
@@ -4541,16 +4541,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-636019.4699837752</v>
+        <v>-765285.932598729</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E5" t="n">
-        <v>-373486.6604214054</v>
+        <v>-424368.29457138</v>
       </c>
     </row>
     <row r="6">
@@ -4558,16 +4558,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-571119.5240670634</v>
+        <v>-678420.3329847984</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E6" t="n">
-        <v>-308586.7145046936</v>
+        <v>-337502.6949574493</v>
       </c>
     </row>
     <row r="7">
@@ -4575,16 +4575,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-506219.5781503516</v>
+        <v>-591554.7333708677</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>262532.8095623698</v>
+        <v>340917.638027349</v>
       </c>
       <c r="E7" t="n">
-        <v>-243686.7685879819</v>
+        <v>-250637.0953435187</v>
       </c>
     </row>
     <row r="8">
@@ -4592,16 +4592,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-441319.6322336399</v>
+        <v>-504689.1337569371</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>262532.8095623698</v>
+        <v>260486.5272737095</v>
       </c>
       <c r="E8" t="n">
-        <v>-178786.8226712701</v>
+        <v>-244202.6064832275</v>
       </c>
     </row>
     <row r="9">
@@ -4609,16 +4609,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-376419.6863169281</v>
+        <v>-417823.5341430064</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>262532.8095623697</v>
+        <v>180055.41652007</v>
       </c>
       <c r="E9" t="n">
-        <v>-113886.8767545584</v>
+        <v>-237768.1176229363</v>
       </c>
     </row>
     <row r="10">
@@ -4626,16 +4626,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-311519.7404002164</v>
+        <v>-330957.9345290757</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>262532.8095623697</v>
+        <v>99624.30576643051</v>
       </c>
       <c r="E10" t="n">
-        <v>-48986.93083784665</v>
+        <v>-231333.6287626452</v>
       </c>
     </row>
     <row r="11">
@@ -4643,16 +4643,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-246619.7944835046</v>
+        <v>-244092.3349151451</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>185270.969185332</v>
+        <v>19193.19501279101</v>
       </c>
       <c r="E11" t="n">
-        <v>-61348.82529817268</v>
+        <v>-224899.139902354</v>
       </c>
     </row>
     <row r="12">
@@ -4660,16 +4660,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-181719.8485667929</v>
+        <v>-157226.7353012144</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>108009.1288082942</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E12" t="n">
-        <v>-73710.71975849873</v>
+        <v>-218464.6510420629</v>
       </c>
     </row>
     <row r="13">
@@ -4677,16 +4677,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-116819.9026500812</v>
+        <v>-70361.13568728374</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>30747.28843125639</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E13" t="n">
-        <v>-86072.61421882479</v>
+        <v>-131599.0514281322</v>
       </c>
     </row>
     <row r="14">
@@ -4694,16 +4694,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>-51919.95673336944</v>
+        <v>16504.46392664694</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E14" t="n">
-        <v>-98434.50867915084</v>
+        <v>-44733.45181420155</v>
       </c>
     </row>
     <row r="15">
@@ -4711,16 +4711,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>12979.9891833423</v>
+        <v>103370.0635405776</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E15" t="n">
-        <v>-33534.56276243909</v>
+        <v>42132.14779972911</v>
       </c>
     </row>
     <row r="16">
@@ -4728,16 +4728,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>77879.93510005403</v>
+        <v>190235.6631545083</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E16" t="n">
-        <v>31365.38315427264</v>
+        <v>128997.7474136598</v>
       </c>
     </row>
     <row r="17">
@@ -4745,16 +4745,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>142779.8810167658</v>
+        <v>277101.2627684389</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E17" t="n">
-        <v>96265.32907098439</v>
+        <v>215863.3470275904</v>
       </c>
     </row>
     <row r="18">
@@ -4762,16 +4762,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>207679.8269334775</v>
+        <v>363966.8623823696</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E18" t="n">
-        <v>161165.2749876961</v>
+        <v>302728.9466415211</v>
       </c>
     </row>
     <row r="19">
@@ -4779,16 +4779,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>272579.7728501892</v>
+        <v>450832.4619963002</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E19" t="n">
-        <v>226065.2209044078</v>
+        <v>389594.5462554517</v>
       </c>
     </row>
     <row r="20">
@@ -4796,16 +4796,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>337479.718766901</v>
+        <v>537698.0616102309</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E20" t="n">
-        <v>290965.1668211196</v>
+        <v>476460.1458693824</v>
       </c>
     </row>
     <row r="21">
@@ -4813,16 +4813,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>402379.6646836127</v>
+        <v>624563.6612241615</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E21" t="n">
-        <v>355865.1127378313</v>
+        <v>563325.745483313</v>
       </c>
     </row>
     <row r="22">
@@ -4830,16 +4830,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>467279.6106003244</v>
+        <v>711429.2608380922</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E22" t="n">
-        <v>420765.058654543</v>
+        <v>650191.3450972437</v>
       </c>
     </row>
     <row r="23">
@@ -4847,16 +4847,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>532179.5565170362</v>
+        <v>798294.8604520229</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E23" t="n">
-        <v>485665.0045712548</v>
+        <v>737056.9447111744</v>
       </c>
     </row>
     <row r="24">
@@ -4864,16 +4864,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>597079.5024337479</v>
+        <v>885160.4600659537</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E24" t="n">
-        <v>550564.9504879664</v>
+        <v>823922.5443251051</v>
       </c>
     </row>
     <row r="25">
@@ -4881,16 +4881,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>661979.4483504597</v>
+        <v>972026.0596798842</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E25" t="n">
-        <v>615464.8964046782</v>
+        <v>910788.1439390357</v>
       </c>
     </row>
     <row r="26">
@@ -4898,16 +4898,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>726879.3942671714</v>
+        <v>1058891.659293815</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E26" t="n">
-        <v>680364.8423213901</v>
+        <v>997653.7435529665</v>
       </c>
     </row>
     <row r="27">
@@ -4915,16 +4915,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>791779.3401838831</v>
+        <v>1145757.258907746</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E27" t="n">
-        <v>745264.7882381016</v>
+        <v>1084519.343166897</v>
       </c>
     </row>
     <row r="28">
@@ -4932,16 +4932,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>856679.2861005949</v>
+        <v>1232622.858521676</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E28" t="n">
-        <v>810164.7341548135</v>
+        <v>1171384.942780828</v>
       </c>
     </row>
     <row r="29">
@@ -4949,16 +4949,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>921579.2320173067</v>
+        <v>1319488.458135607</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E29" t="n">
-        <v>875064.6800715253</v>
+        <v>1258250.542394758</v>
       </c>
     </row>
     <row r="30">
@@ -4966,16 +4966,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>986479.1779340184</v>
+        <v>1406354.057749538</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E30" t="n">
-        <v>939964.6259882371</v>
+        <v>1345116.142008689</v>
       </c>
     </row>
     <row r="31">
@@ -4983,16 +4983,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>1051379.12385073</v>
+        <v>1493219.657363468</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E31" t="n">
-        <v>1004864.571904949</v>
+        <v>1431981.74162262</v>
       </c>
     </row>
     <row r="32">
@@ -5000,16 +5000,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>1116279.069767442</v>
+        <v>1580085.256977399</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-46514.55194578139</v>
+        <v>-61237.91574084849</v>
       </c>
       <c r="E32" t="n">
-        <v>1069764.51782166</v>
+        <v>1518847.34123655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push updated RGGI report
</commit_message>
<xml_diff>
--- a/RGGI PnL Output.xlsx
+++ b/RGGI PnL Output.xlsx
@@ -479,16 +479,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-362229.5502555167</v>
+        <v>-608015.4219922652</v>
       </c>
       <c r="E2" t="n">
-        <v>-476529.5502555167</v>
+        <v>-608015.4219922652</v>
       </c>
     </row>
     <row r="3">
@@ -496,16 +496,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-316386.8147894829</v>
+        <v>-517084.9190198983</v>
       </c>
       <c r="E3" t="n">
-        <v>-420686.8147894829</v>
+        <v>-517084.9190198983</v>
       </c>
     </row>
     <row r="4">
@@ -513,16 +513,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-273864.5940455671</v>
+        <v>-433850.8881261189</v>
       </c>
       <c r="E4" t="n">
-        <v>-368164.5940455671</v>
+        <v>-433850.8881261189</v>
       </c>
     </row>
     <row r="5">
@@ -530,16 +530,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-235240.249646235</v>
+        <v>-360371.4899629905</v>
       </c>
       <c r="E5" t="n">
-        <v>-319540.249646235</v>
+        <v>-360371.4899629905</v>
       </c>
     </row>
     <row r="6">
@@ -547,16 +547,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-200309.2890722251</v>
+        <v>-297339.527727391</v>
       </c>
       <c r="E6" t="n">
-        <v>-274609.2890722251</v>
+        <v>-297339.527727391</v>
       </c>
     </row>
     <row r="7">
@@ -564,16 +564,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-168130.5583429246</v>
+        <v>-243851.8482833975</v>
       </c>
       <c r="E7" t="n">
-        <v>-232430.5583429246</v>
+        <v>-243851.8482833975</v>
       </c>
     </row>
     <row r="8">
@@ -581,16 +581,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-137437.0115647068</v>
+        <v>-197819.4863662811</v>
       </c>
       <c r="E8" t="n">
-        <v>-191737.0115647068</v>
+        <v>-197819.4863662811</v>
       </c>
     </row>
     <row r="9">
@@ -598,16 +598,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-107226.0456992088</v>
+        <v>-156820.6600252705</v>
       </c>
       <c r="E9" t="n">
-        <v>-151526.0456992087</v>
+        <v>-156820.6600252705</v>
       </c>
     </row>
     <row r="10">
@@ -615,16 +615,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-77273.22116595269</v>
+        <v>-119028.6832030883</v>
       </c>
       <c r="E10" t="n">
-        <v>-111573.2211659527</v>
+        <v>-119028.6832030883</v>
       </c>
     </row>
     <row r="11">
@@ -632,16 +632,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-48376.0073459126</v>
+        <v>-83863.9511884173</v>
       </c>
       <c r="E11" t="n">
-        <v>-72676.0073459126</v>
+        <v>-83863.9511884173</v>
       </c>
     </row>
     <row r="12">
@@ -649,16 +649,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-22269.09823005228</v>
+        <v>-52175.86916700007</v>
       </c>
       <c r="E12" t="n">
-        <v>-36569.09823005227</v>
+        <v>-52175.86916700007</v>
       </c>
     </row>
     <row r="13">
@@ -666,16 +666,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-1281.608217255403</v>
+        <v>-25963.49722273639</v>
       </c>
       <c r="E13" t="n">
-        <v>-5581.608217255401</v>
+        <v>-25963.49722273639</v>
       </c>
     </row>
     <row r="14">
@@ -683,16 +683,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>12122.69383211937</v>
+        <v>-7801.011206403011</v>
       </c>
       <c r="E14" t="n">
-        <v>17822.69383211937</v>
+        <v>-7801.011206403011</v>
       </c>
     </row>
     <row r="15">
@@ -700,16 +700,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>15778.33989290365</v>
+        <v>-194.3746579362669</v>
       </c>
       <c r="E15" t="n">
-        <v>31478.33989290365</v>
+        <v>-194.3746579362669</v>
       </c>
     </row>
     <row r="16">
@@ -717,16 +717,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>8125.315202389582</v>
+        <v>-5061.328461508921</v>
       </c>
       <c r="E16" t="n">
-        <v>33825.31520238958</v>
+        <v>-5061.328461508921</v>
       </c>
     </row>
     <row r="17">
@@ -734,16 +734,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-11647.84842292179</v>
+        <v>-23438.50359991641</v>
       </c>
       <c r="E17" t="n">
-        <v>24052.15157707821</v>
+        <v>-23438.50359991641</v>
       </c>
     </row>
     <row r="18">
@@ -751,16 +751,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-43611.85883748991</v>
+        <v>-55425.98914322729</v>
       </c>
       <c r="E18" t="n">
-        <v>2088.141162510088</v>
+        <v>-55425.98914322729</v>
       </c>
     </row>
     <row r="19">
@@ -768,16 +768,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-87212.08521065599</v>
+        <v>-100314.5082275465</v>
       </c>
       <c r="E19" t="n">
-        <v>-31512.08521065599</v>
+        <v>-100314.5082275465</v>
       </c>
     </row>
     <row r="20">
@@ -785,16 +785,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-141439.9160921394</v>
+        <v>-156813.9109880786</v>
       </c>
       <c r="E20" t="n">
-        <v>-75739.91609213944</v>
+        <v>-156813.9109880786</v>
       </c>
     </row>
     <row r="21">
@@ -802,16 +802,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-205015.0966406</v>
+        <v>-223306.8687323929</v>
       </c>
       <c r="E21" t="n">
-        <v>-129315.0966406</v>
+        <v>-223306.8687323929</v>
       </c>
     </row>
     <row r="22">
@@ -819,16 +819,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-276548.0564466503</v>
+        <v>-298074.018137013</v>
       </c>
       <c r="E22" t="n">
-        <v>-190848.0564466503</v>
+        <v>-298074.018137013</v>
       </c>
     </row>
     <row r="23">
@@ -836,16 +836,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-354666.05884465</v>
+        <v>-379462.9524502808</v>
       </c>
       <c r="E23" t="n">
-        <v>-258966.05884465</v>
+        <v>-379462.9524502808</v>
       </c>
     </row>
     <row r="24">
@@ -853,16 +853,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-438098.9712516114</v>
+        <v>-465994.9563738405</v>
       </c>
       <c r="E24" t="n">
-        <v>-332398.9712516114</v>
+        <v>-465994.9563738405</v>
       </c>
     </row>
     <row r="25">
@@ -870,16 +870,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-525728.2701677026</v>
+        <v>-556417.024956425</v>
       </c>
       <c r="E25" t="n">
-        <v>-410028.2701677026</v>
+        <v>-556417.024956425</v>
       </c>
     </row>
     <row r="26">
@@ -887,16 +887,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-616606.8168749069</v>
+        <v>-649712.8970714979</v>
       </c>
       <c r="E26" t="n">
-        <v>-490906.8168749069</v>
+        <v>-649712.8970714979</v>
       </c>
     </row>
     <row r="27">
@@ -904,16 +904,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-709957.9628759634</v>
+        <v>-745087.6603309007</v>
       </c>
       <c r="E27" t="n">
-        <v>-574257.9628759634</v>
+        <v>-745087.6603309007</v>
       </c>
     </row>
     <row r="28">
@@ -921,16 +921,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-805161.7933092059</v>
+        <v>-841938.2999796742</v>
       </c>
       <c r="E28" t="n">
-        <v>-659461.7933092059</v>
+        <v>-841938.2999796742</v>
       </c>
     </row>
     <row r="29">
@@ -938,16 +938,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-901734.7313579633</v>
+        <v>-939819.2437144688</v>
       </c>
       <c r="E29" t="n">
-        <v>-746034.7313579633</v>
+        <v>-939819.2437144688</v>
       </c>
     </row>
     <row r="30">
@@ -955,16 +955,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-999306.9524025458</v>
+        <v>-1038408.679978609</v>
       </c>
       <c r="E30" t="n">
-        <v>-833606.9524025458</v>
+        <v>-1038408.679978609</v>
       </c>
     </row>
     <row r="31">
@@ -972,16 +972,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1097600.460763367</v>
+        <v>-1137478.773892827</v>
       </c>
       <c r="E31" t="n">
-        <v>-921900.4607633674</v>
+        <v>-1137478.773892827</v>
       </c>
     </row>
     <row r="32">
@@ -989,16 +989,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1196409.422466083</v>
+        <v>-1236871.030688924</v>
       </c>
       <c r="E32" t="n">
-        <v>-1010709.422466083</v>
+        <v>-1236871.030688924</v>
       </c>
     </row>
   </sheetData>
@@ -1052,16 +1052,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-362255.8157459879</v>
+        <v>-607083.6711008861</v>
       </c>
       <c r="E2" t="n">
-        <v>-476555.8157459879</v>
+        <v>-607083.6711008861</v>
       </c>
     </row>
     <row r="3">
@@ -1069,16 +1069,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-314019.5161553635</v>
+        <v>-513134.2711006302</v>
       </c>
       <c r="E3" t="n">
-        <v>-418319.5161553635</v>
+        <v>-513134.2711006302</v>
       </c>
     </row>
     <row r="4">
@@ -1086,16 +1086,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-268375.3641774958</v>
+        <v>-425976.0834276862</v>
       </c>
       <c r="E4" t="n">
-        <v>-362675.3641774958</v>
+        <v>-425976.0834276862</v>
       </c>
     </row>
     <row r="5">
@@ -1103,16 +1103,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-226905.086325486</v>
+        <v>-348611.2604175693</v>
       </c>
       <c r="E5" t="n">
-        <v>-311205.086325486</v>
+        <v>-348611.2604175693</v>
       </c>
     </row>
     <row r="6">
@@ -1120,16 +1120,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-190667.8280504309</v>
+        <v>-282895.109783117</v>
       </c>
       <c r="E6" t="n">
-        <v>-264967.8280504309</v>
+        <v>-282895.109783117</v>
       </c>
     </row>
     <row r="7">
@@ -1137,16 +1137,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-159486.7282174463</v>
+        <v>-228726.0663800151</v>
       </c>
       <c r="E7" t="n">
-        <v>-223786.7282174463</v>
+        <v>-228726.0663800151</v>
       </c>
     </row>
     <row r="8">
@@ -1154,16 +1154,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-131771.0583102793</v>
+        <v>-184038.9964947673</v>
       </c>
       <c r="E8" t="n">
-        <v>-186071.0583102793</v>
+        <v>-184038.9964947673</v>
       </c>
     </row>
     <row r="9">
@@ -1171,16 +1171,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-105082.0391262707</v>
+        <v>-145624.876701955</v>
       </c>
       <c r="E9" t="n">
-        <v>-149382.0391262707</v>
+        <v>-145624.876701955</v>
       </c>
     </row>
     <row r="10">
@@ -1188,16 +1188,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-77207.46105637682</v>
+        <v>-110397.4030100309</v>
       </c>
       <c r="E10" t="n">
-        <v>-111507.4610563768</v>
+        <v>-110397.4030100309</v>
       </c>
     </row>
     <row r="11">
@@ -1205,16 +1205,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-47235.63357143544</v>
+        <v>-76564.0796859269</v>
       </c>
       <c r="E11" t="n">
-        <v>-71535.63357143544</v>
+        <v>-76564.0796859269</v>
       </c>
     </row>
     <row r="12">
@@ -1222,16 +1222,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-16148.7266899066</v>
+        <v>-44259.8497388644</v>
       </c>
       <c r="E12" t="n">
-        <v>-30448.7266899066</v>
+        <v>-44259.8497388644</v>
       </c>
     </row>
     <row r="13">
@@ -1239,16 +1239,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>13279.6784891942</v>
+        <v>-15471.79102937753</v>
       </c>
       <c r="E13" t="n">
-        <v>8979.678489194204</v>
+        <v>-15471.79102937753</v>
       </c>
     </row>
     <row r="14">
@@ -1256,16 +1256,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>37175.78860599251</v>
+        <v>6620.580257377544</v>
       </c>
       <c r="E14" t="n">
-        <v>42875.78860599251</v>
+        <v>6620.580257377544</v>
       </c>
     </row>
     <row r="15">
@@ -1273,16 +1273,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>51524.68683535456</v>
+        <v>18573.73569487785</v>
       </c>
       <c r="E15" t="n">
-        <v>67224.68683535456</v>
+        <v>18573.73569487785</v>
       </c>
     </row>
     <row r="16">
@@ -1290,16 +1290,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>53043.20584564193</v>
+        <v>17534.74941317584</v>
       </c>
       <c r="E16" t="n">
-        <v>78743.20584564193</v>
+        <v>17534.74941317584</v>
       </c>
     </row>
     <row r="17">
@@ -1307,16 +1307,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>39726.4466025084</v>
+        <v>1788.208730146667</v>
       </c>
       <c r="E17" t="n">
-        <v>75426.4466025084</v>
+        <v>1788.208730146667</v>
       </c>
     </row>
     <row r="18">
@@ -1324,16 +1324,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>10997.86332893622</v>
+        <v>-29076.39816945436</v>
       </c>
       <c r="E18" t="n">
-        <v>56697.86332893622</v>
+        <v>-29076.39816945436</v>
       </c>
     </row>
     <row r="19">
@@ -1341,16 +1341,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-32466.58737510949</v>
+        <v>-74313.05541229132</v>
       </c>
       <c r="E19" t="n">
-        <v>23233.41262489051</v>
+        <v>-74313.05541229132</v>
       </c>
     </row>
     <row r="20">
@@ -1358,16 +1358,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-89100.71011467336</v>
+        <v>-132351.4275373007</v>
       </c>
       <c r="E20" t="n">
-        <v>-23400.71011467336</v>
+        <v>-132351.4275373007</v>
       </c>
     </row>
     <row r="21">
@@ -1375,16 +1375,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-156856.7828819193</v>
+        <v>-201178.655513344</v>
       </c>
       <c r="E21" t="n">
-        <v>-81156.78288191929</v>
+        <v>-201178.655513344</v>
       </c>
     </row>
     <row r="22">
@@ -1392,16 +1392,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-233561.2209575579</v>
+        <v>-278674.2058496354</v>
       </c>
       <c r="E22" t="n">
-        <v>-147861.2209575579</v>
+        <v>-278674.2058496354</v>
       </c>
     </row>
     <row r="23">
@@ -1409,16 +1409,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-317168.8684069329</v>
+        <v>-362850.05187899</v>
       </c>
       <c r="E23" t="n">
-        <v>-221468.8684069329</v>
+        <v>-362850.05187899</v>
       </c>
     </row>
     <row r="24">
@@ -1426,16 +1426,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-405909.4375050354</v>
+        <v>-451988.8435148868</v>
       </c>
       <c r="E24" t="n">
-        <v>-300209.4375050354</v>
+        <v>-451988.8435148868</v>
       </c>
     </row>
     <row r="25">
@@ -1443,16 +1443,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-498344.576494629</v>
+        <v>-544697.0677849774</v>
       </c>
       <c r="E25" t="n">
-        <v>-382644.576494629</v>
+        <v>-544697.0677849774</v>
       </c>
     </row>
     <row r="26">
@@ -1460,16 +1460,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-593363.3967805482</v>
+        <v>-639899.5248764256</v>
       </c>
       <c r="E26" t="n">
-        <v>-467663.3967805482</v>
+        <v>-639899.5248764256</v>
       </c>
     </row>
     <row r="27">
@@ -1477,16 +1477,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-690143.1947411706</v>
+        <v>-736800.6195874116</v>
       </c>
       <c r="E27" t="n">
-        <v>-554443.1947411706</v>
+        <v>-736800.6195874116</v>
       </c>
     </row>
     <row r="28">
@@ -1494,16 +1494,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-788095.9747245209</v>
+        <v>-834832.1990431675</v>
       </c>
       <c r="E28" t="n">
-        <v>-642395.9747245209</v>
+        <v>-834832.1990431675</v>
       </c>
     </row>
     <row r="29">
@@ -1511,16 +1511,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-886814.1500045825</v>
+        <v>-933600.7666792932</v>
       </c>
       <c r="E29" t="n">
-        <v>-731114.1500045825</v>
+        <v>-933600.7666792932</v>
       </c>
     </row>
     <row r="30">
@@ -1528,16 +1528,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-986022.6095691831</v>
+        <v>-1032840.964115012</v>
       </c>
       <c r="E30" t="n">
-        <v>-820322.6095691831</v>
+        <v>-1032840.964115012</v>
       </c>
     </row>
     <row r="31">
@@ -1545,16 +1545,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1085539.945421518</v>
+        <v>-1132377.986627994</v>
       </c>
       <c r="E31" t="n">
-        <v>-909839.9454215176</v>
+        <v>-1132377.986627994</v>
       </c>
     </row>
     <row r="32">
@@ -1562,16 +1562,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1185248.977442214</v>
+        <v>-1232099.039241985</v>
       </c>
       <c r="E32" t="n">
-        <v>-999548.9774422136</v>
+        <v>-1232099.039241985</v>
       </c>
     </row>
   </sheetData>
@@ -1625,16 +1625,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -1642,16 +1642,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -1659,16 +1659,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -1676,16 +1676,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -1693,16 +1693,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -1710,16 +1710,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -1727,16 +1727,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -1744,16 +1744,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -1761,16 +1761,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -1778,16 +1778,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -1795,16 +1795,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -1812,16 +1812,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -1829,16 +1829,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -1846,16 +1846,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -1863,16 +1863,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -1880,16 +1880,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -1897,16 +1897,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -1914,16 +1914,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -1931,16 +1931,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -1948,16 +1948,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -1965,16 +1965,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -1982,16 +1982,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -1999,16 +1999,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -2016,16 +2016,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -2033,16 +2033,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -2050,16 +2050,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -2067,16 +2067,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -2084,16 +2084,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -2101,16 +2101,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -2118,16 +2118,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -2135,16 +2135,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>
@@ -2198,16 +2198,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -2215,16 +2215,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -2232,16 +2232,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -2249,16 +2249,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -2266,16 +2266,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -2283,16 +2283,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -2300,16 +2300,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -2317,16 +2317,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -2334,16 +2334,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -2351,16 +2351,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -2368,16 +2368,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -2385,16 +2385,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -2402,16 +2402,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -2419,16 +2419,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -2436,16 +2436,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -2453,16 +2453,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -2470,16 +2470,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -2487,16 +2487,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -2504,16 +2504,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -2521,16 +2521,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -2538,16 +2538,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -2555,16 +2555,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -2572,16 +2572,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -2589,16 +2589,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -2606,16 +2606,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -2623,16 +2623,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -2640,16 +2640,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -2657,16 +2657,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -2674,16 +2674,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -2691,16 +2691,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -2708,16 +2708,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>
@@ -2771,16 +2771,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -2788,16 +2788,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -2805,16 +2805,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -2822,16 +2822,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -2839,16 +2839,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -2856,16 +2856,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -2873,16 +2873,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -2890,16 +2890,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -2907,16 +2907,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -2924,16 +2924,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -2941,16 +2941,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -2958,16 +2958,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -2975,16 +2975,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -2992,16 +2992,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -3009,16 +3009,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -3026,16 +3026,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -3043,16 +3043,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -3060,16 +3060,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -3077,16 +3077,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -3094,16 +3094,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -3111,16 +3111,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -3128,16 +3128,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -3145,16 +3145,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -3162,16 +3162,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -3179,16 +3179,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -3196,16 +3196,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -3213,16 +3213,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -3230,16 +3230,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -3247,16 +3247,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -3264,16 +3264,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -3281,16 +3281,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>
@@ -3344,16 +3344,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -3361,16 +3361,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -3378,16 +3378,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -3395,16 +3395,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -3412,16 +3412,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -3429,16 +3429,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -3446,16 +3446,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -3463,16 +3463,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -3480,16 +3480,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -3497,16 +3497,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -3514,16 +3514,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -3531,16 +3531,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -3548,16 +3548,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -3565,16 +3565,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -3582,16 +3582,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -3599,16 +3599,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -3616,16 +3616,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -3633,16 +3633,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -3650,16 +3650,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -3667,16 +3667,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -3684,16 +3684,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -3701,16 +3701,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -3718,16 +3718,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -3735,16 +3735,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -3752,16 +3752,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -3769,16 +3769,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -3786,16 +3786,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -3803,16 +3803,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -3820,16 +3820,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -3837,16 +3837,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -3854,16 +3854,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>
@@ -3917,16 +3917,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -3934,16 +3934,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -3951,16 +3951,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -3968,16 +3968,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -3985,16 +3985,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -4002,16 +4002,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -4019,16 +4019,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -4036,16 +4036,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -4053,16 +4053,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -4070,16 +4070,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -4087,16 +4087,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -4104,16 +4104,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -4121,16 +4121,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -4138,16 +4138,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -4155,16 +4155,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -4172,16 +4172,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -4189,16 +4189,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -4206,16 +4206,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -4223,16 +4223,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -4240,16 +4240,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -4257,16 +4257,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -4274,16 +4274,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -4291,16 +4291,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -4308,16 +4308,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -4325,16 +4325,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -4342,16 +4342,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -4359,16 +4359,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -4376,16 +4376,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -4393,16 +4393,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -4410,16 +4410,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -4427,16 +4427,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>
@@ -4490,16 +4490,16 @@
         <v>10</v>
       </c>
       <c r="B2" t="n">
-        <v>-114300</v>
+        <v>-0</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-365986.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E2" t="n">
-        <v>-480286.0925968389</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="3">
@@ -4507,16 +4507,16 @@
         <v>11</v>
       </c>
       <c r="B3" t="n">
-        <v>-104300</v>
+        <v>-0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-315986.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
       <c r="E3" t="n">
-        <v>-420286.0925968389</v>
+        <v>-512852.6396494271</v>
       </c>
     </row>
     <row r="4">
@@ -4524,16 +4524,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="n">
-        <v>-94300</v>
+        <v>-0</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-265986.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
       <c r="E4" t="n">
-        <v>-360286.0925968389</v>
+        <v>-412852.6396494271</v>
       </c>
     </row>
     <row r="5">
@@ -4541,16 +4541,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>-84300</v>
+        <v>-0</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-215986.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
       <c r="E5" t="n">
-        <v>-300286.0925968389</v>
+        <v>-312852.6396494273</v>
       </c>
     </row>
     <row r="6">
@@ -4558,16 +4558,16 @@
         <v>14</v>
       </c>
       <c r="B6" t="n">
-        <v>-74300</v>
+        <v>-0</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
       <c r="E6" t="n">
-        <v>-240286.0925968389</v>
+        <v>-212852.6396494273</v>
       </c>
     </row>
     <row r="7">
@@ -4575,16 +4575,16 @@
         <v>15</v>
       </c>
       <c r="B7" t="n">
-        <v>-64300</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E7" t="n">
-        <v>-180286.0925968389</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="8">
@@ -4592,16 +4592,16 @@
         <v>16</v>
       </c>
       <c r="B8" t="n">
-        <v>-54300</v>
+        <v>-0</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E8" t="n">
-        <v>-120286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="9">
@@ -4609,16 +4609,16 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>-44300</v>
+        <v>-0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-15986.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
       <c r="E9" t="n">
-        <v>-60286.09259683892</v>
+        <v>87147.36035057277</v>
       </c>
     </row>
     <row r="10">
@@ -4626,16 +4626,16 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>-34300</v>
+        <v>-0</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>-65986.09259683892</v>
+        <v>-12852.63964942723</v>
       </c>
       <c r="E10" t="n">
-        <v>-100286.0925968389</v>
+        <v>-12852.63964942723</v>
       </c>
     </row>
     <row r="11">
@@ -4643,16 +4643,16 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>-24300</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-115986.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E11" t="n">
-        <v>-140286.0925968389</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="12">
@@ -4660,16 +4660,16 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>-14300</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-165986.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
       <c r="E12" t="n">
-        <v>-180286.0925968389</v>
+        <v>-212852.6396494272</v>
       </c>
     </row>
     <row r="13">
@@ -4677,16 +4677,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>-4299.999999999997</v>
+        <v>-0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-65986.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
       <c r="E13" t="n">
-        <v>-70286.09259683892</v>
+        <v>-112852.6396494272</v>
       </c>
     </row>
     <row r="14">
@@ -4694,16 +4694,16 @@
         <v>22</v>
       </c>
       <c r="B14" t="n">
-        <v>5700.000000000003</v>
+        <v>-0</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>34013.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E14" t="n">
-        <v>39713.90740316109</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="15">
@@ -4711,16 +4711,16 @@
         <v>23</v>
       </c>
       <c r="B15" t="n">
-        <v>15700</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E15" t="n">
-        <v>149713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="16">
@@ -4728,16 +4728,16 @@
         <v>24</v>
       </c>
       <c r="B16" t="n">
-        <v>25700</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E16" t="n">
-        <v>259713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="17">
@@ -4745,16 +4745,16 @@
         <v>25</v>
       </c>
       <c r="B17" t="n">
-        <v>35700</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>334013.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
       <c r="E17" t="n">
-        <v>369713.9074031611</v>
+        <v>287147.3603505728</v>
       </c>
     </row>
     <row r="18">
@@ -4762,16 +4762,16 @@
         <v>26</v>
       </c>
       <c r="B18" t="n">
-        <v>45700</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>234013.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
       <c r="E18" t="n">
-        <v>279713.9074031611</v>
+        <v>187147.3603505728</v>
       </c>
     </row>
     <row r="19">
@@ -4779,16 +4779,16 @@
         <v>27</v>
       </c>
       <c r="B19" t="n">
-        <v>55700</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>134013.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
       <c r="E19" t="n">
-        <v>189713.9074031611</v>
+        <v>87147.3603505728</v>
       </c>
     </row>
     <row r="20">
@@ -4796,16 +4796,16 @@
         <v>28</v>
       </c>
       <c r="B20" t="n">
-        <v>65700</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>34013.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
       <c r="E20" t="n">
-        <v>99713.90740316111</v>
+        <v>-12852.6396494272</v>
       </c>
     </row>
     <row r="21">
@@ -4813,16 +4813,16 @@
         <v>29</v>
       </c>
       <c r="B21" t="n">
-        <v>75700</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-65986.09259683883</v>
+        <v>-112852.6396494273</v>
       </c>
       <c r="E21" t="n">
-        <v>9713.907403161167</v>
+        <v>-112852.6396494273</v>
       </c>
     </row>
     <row r="22">
@@ -4830,16 +4830,16 @@
         <v>30</v>
       </c>
       <c r="B22" t="n">
-        <v>85700</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-165986.0925968388</v>
+        <v>-212852.6396494274</v>
       </c>
       <c r="E22" t="n">
-        <v>-80286.09259683883</v>
+        <v>-212852.6396494274</v>
       </c>
     </row>
     <row r="23">
@@ -4847,16 +4847,16 @@
         <v>31</v>
       </c>
       <c r="B23" t="n">
-        <v>95700</v>
+        <v>0</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-265986.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
       <c r="E23" t="n">
-        <v>-170286.0925968388</v>
+        <v>-312852.6396494274</v>
       </c>
     </row>
     <row r="24">
@@ -4864,16 +4864,16 @@
         <v>32</v>
       </c>
       <c r="B24" t="n">
-        <v>105700</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-365986.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
       <c r="E24" t="n">
-        <v>-260286.0925968388</v>
+        <v>-412852.6396494274</v>
       </c>
     </row>
     <row r="25">
@@ -4881,16 +4881,16 @@
         <v>33</v>
       </c>
       <c r="B25" t="n">
-        <v>115700</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-465986.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
       <c r="E25" t="n">
-        <v>-350286.0925968388</v>
+        <v>-512852.6396494274</v>
       </c>
     </row>
     <row r="26">
@@ -4898,16 +4898,16 @@
         <v>34</v>
       </c>
       <c r="B26" t="n">
-        <v>125700</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-565986.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
       <c r="E26" t="n">
-        <v>-440286.0925968387</v>
+        <v>-612852.6396494271</v>
       </c>
     </row>
     <row r="27">
@@ -4915,16 +4915,16 @@
         <v>35</v>
       </c>
       <c r="B27" t="n">
-        <v>135700</v>
+        <v>0</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-665986.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
       <c r="E27" t="n">
-        <v>-530286.0925968387</v>
+        <v>-712852.639649427</v>
       </c>
     </row>
     <row r="28">
@@ -4932,16 +4932,16 @@
         <v>36</v>
       </c>
       <c r="B28" t="n">
-        <v>145700</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-765986.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
       <c r="E28" t="n">
-        <v>-620286.0925968387</v>
+        <v>-812852.639649427</v>
       </c>
     </row>
     <row r="29">
@@ -4949,16 +4949,16 @@
         <v>37</v>
       </c>
       <c r="B29" t="n">
-        <v>155700</v>
+        <v>0</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-865986.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
       <c r="E29" t="n">
-        <v>-710286.0925968387</v>
+        <v>-912852.639649427</v>
       </c>
     </row>
     <row r="30">
@@ -4966,16 +4966,16 @@
         <v>38</v>
       </c>
       <c r="B30" t="n">
-        <v>165700</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-965986.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
       <c r="E30" t="n">
-        <v>-800286.0925968387</v>
+        <v>-1012852.639649427</v>
       </c>
     </row>
     <row r="31">
@@ -4983,16 +4983,16 @@
         <v>39</v>
       </c>
       <c r="B31" t="n">
-        <v>175700</v>
+        <v>0</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-1065986.092596839</v>
+        <v>-1112852.639649427</v>
       </c>
       <c r="E31" t="n">
-        <v>-890286.0925968387</v>
+        <v>-1112852.639649427</v>
       </c>
     </row>
     <row r="32">
@@ -5000,16 +5000,16 @@
         <v>40</v>
       </c>
       <c r="B32" t="n">
-        <v>185700</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-1165986.092596839</v>
+        <v>-1212852.639649427</v>
       </c>
       <c r="E32" t="n">
-        <v>-980286.0925968387</v>
+        <v>-1212852.639649427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>